<commit_message>
updated project with Selenium 4.14.0
Signed-off-by: niteshkarhe <nitesh.karhe@gmail.com>
</commit_message>
<xml_diff>
--- a/crmpro_automation/testdata/contact_pg_testdata.xlsx
+++ b/crmpro_automation/testdata/contact_pg_testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NK\Python\PyTestFramework\crmpro_automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NK\PythonProject\PyTestFramework\crmpro_automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>TestCase</t>
   </si>
@@ -605,18 +605,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,9 +654,8 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -692,10 +692,11 @@
       <c r="L2" s="1">
         <v>1992</v>
       </c>
-      <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -729,11 +730,8 @@
       <c r="L3" s="1">
         <v>1980</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -770,11 +768,8 @@
       <c r="L4" s="1">
         <v>1992</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>22</v>
       </c>

</xml_diff>